<commit_message>
Updated log until 9th march
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>PU1</t>
   </si>
@@ -108,10 +108,19 @@
     <t>Show papermodel to studass</t>
   </si>
   <si>
-    <t>KTN Implementation user and server</t>
-  </si>
-  <si>
     <t>Implementation of helper classes for all sections.</t>
+  </si>
+  <si>
+    <t>KTN Implementation user and server login</t>
+  </si>
+  <si>
+    <t>MMI Report</t>
+  </si>
+  <si>
+    <t>Java fx installation and understanding…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB: Implementation of database in java. </t>
   </si>
 </sst>
 </file>
@@ -468,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -645,7 +654,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:O3" si="0">SUM(B6:B30)</f>
+        <f t="shared" ref="B3:O3" si="0">SUM(B6:B32)</f>
         <v>10</v>
       </c>
       <c r="C3" s="4">
@@ -673,16 +682,16 @@
         <v>30</v>
       </c>
       <c r="I3" s="4">
-        <f>SUM(I5:I30)</f>
+        <f>SUM(I5:I32)</f>
         <v>29</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(J5:J30)</f>
+        <f>SUM(J5:J32)</f>
         <v>27</v>
       </c>
       <c r="K3" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="L3" s="4">
         <f t="shared" si="0"/>
@@ -727,6 +736,9 @@
       <c r="J5">
         <v>1</v>
       </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
@@ -843,7 +855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -854,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -862,7 +874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -870,7 +882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -878,34 +890,61 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J22">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30">
-      <c r="A29" s="3" t="s">
+    <row r="31" spans="1:11" ht="30">
+      <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" t="s">
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated timesheet until 11th march
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>PU1</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t xml:space="preserve">DB: Implementation of database in java. </t>
+  </si>
+  <si>
+    <t>New requirment mail</t>
+  </si>
+  <si>
+    <t>Java fx screen design</t>
   </si>
 </sst>
 </file>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -654,7 +660,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:O3" si="0">SUM(B6:B32)</f>
+        <f t="shared" ref="B3:O3" si="0">SUM(B6:B33)</f>
         <v>10</v>
       </c>
       <c r="C3" s="4">
@@ -682,11 +688,11 @@
         <v>30</v>
       </c>
       <c r="I3" s="4">
-        <f>SUM(I5:I32)</f>
+        <f>SUM(I5:I33)</f>
         <v>29</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(J5:J32)</f>
+        <f>SUM(J5:J33)</f>
         <v>27</v>
       </c>
       <c r="K3" s="4">
@@ -707,7 +713,7 @@
       </c>
       <c r="O3" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -855,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -866,7 +872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -874,7 +880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -882,7 +888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -890,7 +896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -900,8 +906,11 @@
       <c r="K21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="O21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -909,7 +918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -917,7 +926,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -925,26 +934,45 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="O25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" t="s">
         <v>34</v>
       </c>
-      <c r="K25">
+      <c r="K26">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="O26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="O27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:15" ht="30">
+      <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
-      <c r="A32" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Logged hours for tuesday 11.03
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>PU1</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Java fx screen design</t>
+  </si>
+  <si>
+    <t>KTN: JSON in java</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -660,7 +663,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:O3" si="0">SUM(B6:B33)</f>
+        <f t="shared" ref="B3:V3" si="0">SUM(B6:B34)</f>
         <v>10</v>
       </c>
       <c r="C3" s="4">
@@ -688,11 +691,11 @@
         <v>30</v>
       </c>
       <c r="I3" s="4">
-        <f>SUM(I5:I33)</f>
+        <f>SUM(I5:I34)</f>
         <v>29</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(J5:J33)</f>
+        <f>SUM(J5:J34)</f>
         <v>27</v>
       </c>
       <c r="K3" s="4">
@@ -715,13 +718,34 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
+      <c r="P3" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="Q3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -745,6 +769,12 @@
       <c r="K5">
         <v>1</v>
       </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
@@ -861,7 +891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -872,7 +902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -880,7 +910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -888,7 +918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -896,7 +926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -910,7 +940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -918,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -926,7 +956,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -934,15 +964,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>36</v>
       </c>
       <c r="O25">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -952,8 +985,11 @@
       <c r="O26">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="P26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -961,18 +997,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="P28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="30">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:1" ht="30">
+      <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Logged hours for wednesday 12th march
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>PU1</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>KTN: JSON in java</t>
+  </si>
+  <si>
+    <t>KTN: Server and client</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -486,189 +492,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z34"/>
+  <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="53.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>10</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>11</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>12</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>13</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>7</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>41695</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>41696</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>41697</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>41698</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>41699</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>41700</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>41701</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>41702</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>41703</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>41704</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>41705</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>41706</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>41707</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>41708</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>41709</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>41710</v>
       </c>
-      <c r="R2" s="1">
+      <c r="S2" s="1">
         <v>41711</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>41712</v>
       </c>
-      <c r="T2" s="1">
+      <c r="U2" s="1">
         <v>41713</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="1">
         <v>41714</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>41715</v>
       </c>
-      <c r="W2" s="1">
+      <c r="X2" s="1">
         <v>41716</v>
       </c>
-      <c r="X2" s="1">
+      <c r="Y2" s="1">
         <v>41717</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Z2" s="1">
         <v>41718</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AA2" s="1">
         <v>41719</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:V3" si="0">SUM(B6:B34)</f>
+        <f>SUM(C3:W3)</f>
+        <v>333</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:W3" si="0">SUM(C6:C35)</f>
         <v>10</v>
-      </c>
-      <c r="C3" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" si="0"/>
@@ -676,59 +686,59 @@
       </c>
       <c r="E3" s="4">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G3" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H3" s="4">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="I3" s="4">
-        <f>SUM(I5:I34)</f>
+      <c r="J3" s="4">
+        <f>SUM(J5:J35)</f>
         <v>29</v>
       </c>
-      <c r="J3" s="4">
-        <f>SUM(J5:J34)</f>
+      <c r="K3" s="4">
+        <f t="shared" ref="K3:O3" si="1">SUM(K5:K35)</f>
         <v>27</v>
       </c>
-      <c r="K3" s="4">
-        <f t="shared" si="0"/>
+      <c r="L3" s="4">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="M3" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <f>SUM(P5:P35)</f>
         <v>36</v>
       </c>
-      <c r="L3" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N3" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O3" s="4">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="P3" s="4">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
       <c r="Q3" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(Q5:Q35)</f>
+        <v>40</v>
       </c>
       <c r="R3" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(R5:R35)</f>
+        <v>30</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" si="0"/>
@@ -746,277 +756,302 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W3" s="1"/>
+      <c r="W3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:26">
+      <c r="AA3" s="1"/>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:27">
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>2</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
-      <c r="O5">
+      <c r="L5">
         <v>1</v>
       </c>
       <c r="P5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:27">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>30</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>6</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:27">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>24</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>15</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:27">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:27">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:27">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:27">
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:27">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:27">
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="H14">
-        <v>10</v>
-      </c>
       <c r="I14">
         <v>10</v>
       </c>
       <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:27">
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>8</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:27">
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>8</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
         <v>28</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:18">
       <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>2</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>4</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:18">
       <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:18">
       <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:18">
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>14</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
+        <v>25</v>
+      </c>
+      <c r="R25">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
         <v>34</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>7</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>7</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="R26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>35</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:18">
       <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="R28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="R29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="30">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:2" ht="30">
+      <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the log until 16th march
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -495,7 +495,7 @@
   <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -674,7 +674,7 @@
       </c>
       <c r="B3" s="4">
         <f>SUM(C3:W3)</f>
-        <v>333</v>
+        <v>381</v>
       </c>
       <c r="C3" s="4">
         <f t="shared" ref="C3:W3" si="0">SUM(C6:C35)</f>
@@ -742,11 +742,11 @@
       </c>
       <c r="S3" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="T3" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="U3" s="4">
         <f t="shared" si="0"/>
@@ -792,6 +792,9 @@
       <c r="R5">
         <v>1</v>
       </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:27">
       <c r="A6" t="s">
@@ -908,7 +911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:20">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -919,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:20">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -927,7 +930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:20">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -935,7 +938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:20">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -943,7 +946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:20">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -957,7 +960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:20">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -965,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:20">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -973,7 +976,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:20">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -981,7 +984,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:20">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -994,8 +997,14 @@
       <c r="R25">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="S25">
+        <v>12</v>
+      </c>
+      <c r="T25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1011,8 +1020,14 @@
       <c r="R26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:18">
+      <c r="S26">
+        <v>6</v>
+      </c>
+      <c r="T26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1020,7 +1035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:20">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1031,15 +1046,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:20">
       <c r="A29" t="s">
         <v>38</v>
       </c>
       <c r="R29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:18">
+      <c r="S29">
+        <v>6</v>
+      </c>
+      <c r="T29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Updated the log until 17th march
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>PU1</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>Få folk</t>
+  </si>
+  <si>
+    <t>KTN: Functionality for GUI class</t>
+  </si>
+  <si>
+    <t>Java fx: Main screen</t>
+  </si>
+  <si>
+    <t>Mail class:</t>
+  </si>
+  <si>
+    <t>Java fx: Viewscreen and logic</t>
   </si>
 </sst>
 </file>
@@ -496,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA35"/>
+  <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -678,10 +690,10 @@
       </c>
       <c r="B3" s="4">
         <f>SUM(C3:W3)</f>
-        <v>381</v>
+        <v>411</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:W3" si="0">SUM(C6:C35)</f>
+        <f t="shared" ref="C3:W3" si="0">SUM(C6:C39)</f>
         <v>10</v>
       </c>
       <c r="D3" s="4">
@@ -709,11 +721,11 @@
         <v>30</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(J5:J35)</f>
+        <f>SUM(J5:J39)</f>
         <v>29</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:O3" si="1">SUM(K5:K35)</f>
+        <f t="shared" ref="K3:O3" si="1">SUM(K5:K39)</f>
         <v>27</v>
       </c>
       <c r="L3" s="4">
@@ -733,15 +745,15 @@
         <v>0</v>
       </c>
       <c r="P3" s="4">
-        <f>SUM(P5:P35)</f>
+        <f>SUM(P5:P39)</f>
         <v>36</v>
       </c>
       <c r="Q3" s="4">
-        <f>SUM(Q5:Q35)</f>
+        <f>SUM(Q5:Q39)</f>
         <v>40</v>
       </c>
       <c r="R3" s="4">
-        <f>SUM(R5:R35)</f>
+        <f>SUM(R5:R39)</f>
         <v>30</v>
       </c>
       <c r="S3" s="6">
@@ -762,7 +774,7 @@
       </c>
       <c r="W3" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -918,7 +930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -929,7 +941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -937,7 +949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -945,7 +957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -953,7 +965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -967,7 +979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -975,7 +987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -983,7 +995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -991,7 +1003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1011,7 +1023,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1033,8 +1045,11 @@
       <c r="T26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:20">
+      <c r="W26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1042,7 +1057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1053,7 +1068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1067,19 +1082,51 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="W30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="W31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="W32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="W33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30">
-      <c r="A34" s="3" t="s">
+    <row r="38" spans="1:23" ht="30">
+      <c r="A38" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:23">
+      <c r="A39" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated log for 18th march
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
@@ -11,12 +11,12 @@
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>PU1</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Java fx: Viewscreen and logic</t>
+  </si>
+  <si>
+    <t>Java fx: Editscreen</t>
   </si>
 </sst>
 </file>
@@ -508,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA39"/>
+  <dimension ref="A1:AA40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+      <selection activeCell="W46" sqref="W46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -693,7 +696,7 @@
         <v>411</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:W3" si="0">SUM(C6:C39)</f>
+        <f t="shared" ref="C3:W3" si="0">SUM(C6:C40)</f>
         <v>10</v>
       </c>
       <c r="D3" s="4">
@@ -721,11 +724,11 @@
         <v>30</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(J5:J39)</f>
+        <f>SUM(J5:J40)</f>
         <v>29</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:O3" si="1">SUM(K5:K39)</f>
+        <f t="shared" ref="K3:O3" si="1">SUM(K5:K40)</f>
         <v>27</v>
       </c>
       <c r="L3" s="4">
@@ -745,15 +748,15 @@
         <v>0</v>
       </c>
       <c r="P3" s="4">
-        <f>SUM(P5:P39)</f>
+        <f>SUM(P5:P40)</f>
         <v>36</v>
       </c>
       <c r="Q3" s="4">
-        <f>SUM(Q5:Q39)</f>
+        <f>SUM(Q5:Q40)</f>
         <v>40</v>
       </c>
       <c r="R3" s="4">
-        <f>SUM(R5:R39)</f>
+        <f>SUM(R5:R40)</f>
         <v>30</v>
       </c>
       <c r="S3" s="6">
@@ -930,7 +933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:24">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -941,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:24">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -949,7 +952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:24">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -957,7 +960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:24">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -965,7 +968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:24">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -979,7 +982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:24">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -987,7 +990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:24">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -995,7 +998,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:24">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:24">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:24">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1048,8 +1051,11 @@
       <c r="W26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:23">
+      <c r="X26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:24">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:24">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1082,51 +1088,68 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:24">
       <c r="A30" t="s">
         <v>41</v>
       </c>
       <c r="W30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:23">
+      <c r="X30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
       <c r="A31" t="s">
         <v>42</v>
       </c>
       <c r="W31">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:23">
+      <c r="X31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24">
       <c r="A32" t="s">
         <v>44</v>
       </c>
       <c r="W32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:23">
+      <c r="X32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24">
       <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="X33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
+      <c r="A34" t="s">
         <v>43</v>
       </c>
-      <c r="W33">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23">
-      <c r="A34" t="s">
+      <c r="W34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24">
+      <c r="A35" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="30">
-      <c r="A38" s="3" t="s">
+    <row r="39" spans="1:24" ht="30">
+      <c r="A39" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="1:23">
-      <c r="A39" t="s">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:24">
+      <c r="A40" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated log until 20th march
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>PU1</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Java fx: Editscreen</t>
+  </si>
+  <si>
+    <t>Integration database and network</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA40"/>
+  <dimension ref="A1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W46" sqref="W46"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -696,7 +699,7 @@
         <v>411</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:W3" si="0">SUM(C6:C40)</f>
+        <f t="shared" ref="C3:AA3" si="0">SUM(C6:C41)</f>
         <v>10</v>
       </c>
       <c r="D3" s="4">
@@ -724,11 +727,11 @@
         <v>30</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(J5:J40)</f>
+        <f>SUM(J5:J41)</f>
         <v>29</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:O3" si="1">SUM(K5:K40)</f>
+        <f t="shared" ref="K3:O3" si="1">SUM(K5:K41)</f>
         <v>27</v>
       </c>
       <c r="L3" s="4">
@@ -748,15 +751,15 @@
         <v>0</v>
       </c>
       <c r="P3" s="4">
-        <f>SUM(P5:P40)</f>
+        <f>SUM(P5:P41)</f>
         <v>36</v>
       </c>
       <c r="Q3" s="4">
-        <f>SUM(Q5:Q40)</f>
+        <f>SUM(Q5:Q41)</f>
         <v>40</v>
       </c>
       <c r="R3" s="4">
-        <f>SUM(R5:R40)</f>
+        <f>SUM(R5:R41)</f>
         <v>30</v>
       </c>
       <c r="S3" s="6">
@@ -779,10 +782,22 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
+      <c r="X3" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="Y3" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="Z3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:27">
       <c r="A4" t="s">
@@ -933,7 +948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -944,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -952,7 +967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -960,7 +975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -968,7 +983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -982,7 +997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -990,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -998,7 +1013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1006,7 +1021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1026,7 +1041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1054,8 +1069,11 @@
       <c r="X26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:24">
+      <c r="Y26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1063,7 +1081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1074,7 +1092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1088,7 +1106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1099,7 +1117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1109,8 +1127,11 @@
       <c r="X31">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:24">
+      <c r="Y31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1120,16 +1141,22 @@
       <c r="X32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:24">
+      <c r="Y32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
       <c r="X33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:24">
+      <c r="Y33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -1137,19 +1164,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:25">
       <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="X35">
+        <v>2</v>
+      </c>
+      <c r="Y35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
+      <c r="A36" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="30">
-      <c r="A39" s="3" t="s">
+    <row r="40" spans="1:25" ht="30">
+      <c r="A40" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:24">
-      <c r="A40" t="s">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:25">
+      <c r="A41" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented getStatusForAppointment and getLoggedInUser
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -517,7 +517,7 @@
   <dimension ref="A1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -695,8 +695,8 @@
         <v>19</v>
       </c>
       <c r="B3" s="4">
-        <f>SUM(C3:W3)</f>
-        <v>411</v>
+        <f>SUM(C3:AA3)</f>
+        <v>479</v>
       </c>
       <c r="C3" s="4">
         <f t="shared" ref="C3:AA3" si="0">SUM(C6:C41)</f>

</xml_diff>

<commit_message>
Added a diagram of hours per day worked
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>PU1</t>
   </si>
@@ -157,6 +157,21 @@
   </si>
   <si>
     <t>Integration database and network</t>
+  </si>
+  <si>
+    <t>Integration and testing GUI and backend: Calendar screen</t>
+  </si>
+  <si>
+    <t>Integration and testing GUI and backend: View appointment</t>
+  </si>
+  <si>
+    <t>Integration and testing GUI and backend: Edit appointment</t>
+  </si>
+  <si>
+    <t>PU 5:</t>
+  </si>
+  <si>
+    <t>D3:</t>
   </si>
 </sst>
 </file>
@@ -227,6 +242,285 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nb-NO"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.3196850393700792E-2"/>
+          <c:y val="2.8229334292984517E-2"/>
+          <c:w val="0.69181692913385828"/>
+          <c:h val="0.67822995350111204"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Hours per day</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Ark1'!$C$2:$AA$2</c:f>
+              <c:numCache>
+                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>41695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41697</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41701</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41703</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41704</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41705</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41706</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41707</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41708</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41709</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41710</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41711</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41712</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41713</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41714</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41715</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41716</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41717</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41718</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41719</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$C$3:$AA$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="92144768"/>
+        <c:axId val="92146304"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="92144768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="dd/mm/yyyy" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92146304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="92146304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92144768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>449211</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>20463</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57005</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>177346</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -514,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA41"/>
+  <dimension ref="A1:AA46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R43" sqref="R43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -696,10 +990,10 @@
       </c>
       <c r="B3" s="4">
         <f>SUM(C3:AA3)</f>
-        <v>479</v>
+        <v>567</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:AA3" si="0">SUM(C6:C41)</f>
+        <f t="shared" ref="C3:AA3" si="0">SUM(C6:C46)</f>
         <v>10</v>
       </c>
       <c r="D3" s="4">
@@ -727,11 +1021,11 @@
         <v>30</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(J5:J41)</f>
+        <f>SUM(J5:J46)</f>
         <v>29</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:O3" si="1">SUM(K5:K41)</f>
+        <f t="shared" ref="K3:O3" si="1">SUM(K5:K46)</f>
         <v>27</v>
       </c>
       <c r="L3" s="4">
@@ -751,20 +1045,20 @@
         <v>0</v>
       </c>
       <c r="P3" s="4">
-        <f>SUM(P5:P41)</f>
+        <f>SUM(P5:P46)</f>
         <v>36</v>
       </c>
       <c r="Q3" s="4">
-        <f>SUM(Q5:Q41)</f>
+        <f>SUM(Q5:Q46)</f>
         <v>40</v>
       </c>
       <c r="R3" s="4">
-        <f>SUM(R5:R41)</f>
+        <f>SUM(R5:R46)</f>
         <v>30</v>
       </c>
       <c r="S3" s="6">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="T3" s="6">
         <f t="shared" si="0"/>
@@ -788,21 +1082,25 @@
       </c>
       <c r="Y3" s="4">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Z3" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AA3" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="4">
+        <f t="shared" ref="B4:B40" si="2">SUM(C4:AA4)</f>
+        <v>0</v>
+      </c>
       <c r="S4" t="s">
         <v>40</v>
       </c>
@@ -811,6 +1109,10 @@
       <c r="A5" t="s">
         <v>21</v>
       </c>
+      <c r="B5" s="4">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="J5">
         <v>2</v>
       </c>
@@ -830,6 +1132,9 @@
         <v>1</v>
       </c>
       <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
         <v>1</v>
       </c>
     </row>
@@ -837,6 +1142,10 @@
       <c r="A6" t="s">
         <v>22</v>
       </c>
+      <c r="B6" s="4">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
       <c r="C6">
         <v>10</v>
       </c>
@@ -845,6 +1154,10 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
+      <c r="B7" s="4">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
       <c r="D7">
         <v>30</v>
       </c>
@@ -862,6 +1175,10 @@
       <c r="A8" t="s">
         <v>2</v>
       </c>
+      <c r="B8" s="4">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
       <c r="E8">
         <v>24</v>
       </c>
@@ -879,6 +1196,10 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
+      <c r="B9" s="4">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
       <c r="F9" s="2">
         <v>10</v>
       </c>
@@ -887,6 +1208,10 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
+      <c r="B10" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="F10">
         <v>5</v>
       </c>
@@ -895,6 +1220,10 @@
       <c r="A11" t="s">
         <v>15</v>
       </c>
+      <c r="B11" s="4">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="F11">
         <v>2</v>
       </c>
@@ -903,6 +1232,10 @@
       <c r="A12" t="s">
         <v>24</v>
       </c>
+      <c r="B12" s="4">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
       <c r="I12">
         <v>4</v>
       </c>
@@ -911,6 +1244,10 @@
       <c r="A13" t="s">
         <v>16</v>
       </c>
+      <c r="B13" s="4">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
       <c r="I13" s="5">
         <v>4</v>
       </c>
@@ -919,6 +1256,10 @@
       <c r="A14" t="s">
         <v>17</v>
       </c>
+      <c r="B14" s="4">
+        <f>SUM(C14:AA14)</f>
+        <v>26</v>
+      </c>
       <c r="I14">
         <v>10</v>
       </c>
@@ -933,6 +1274,10 @@
       <c r="A15" t="s">
         <v>20</v>
       </c>
+      <c r="B15" s="4">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
       <c r="I15">
         <v>8</v>
       </c>
@@ -944,14 +1289,22 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
+      <c r="B16" s="4">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
       <c r="I16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:27">
       <c r="A17" t="s">
         <v>25</v>
       </c>
+      <c r="B17" s="4">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="J17">
         <v>8</v>
       </c>
@@ -959,34 +1312,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:27">
       <c r="A18" t="s">
         <v>29</v>
       </c>
+      <c r="B18" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="J18">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:27">
       <c r="A19" t="s">
         <v>27</v>
       </c>
+      <c r="B19" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="K19">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:27">
       <c r="A20" t="s">
         <v>28</v>
       </c>
+      <c r="B20" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="K20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:27">
       <c r="A21" t="s">
         <v>31</v>
       </c>
+      <c r="B21" s="4">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
       <c r="K21">
         <v>2</v>
       </c>
@@ -997,34 +1366,50 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:27">
       <c r="A22" t="s">
         <v>30</v>
       </c>
+      <c r="B22" s="4">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="K22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:27">
       <c r="A23" t="s">
         <v>32</v>
       </c>
+      <c r="B23" s="4">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
       <c r="L23">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:27">
       <c r="A24" t="s">
         <v>33</v>
       </c>
+      <c r="B24" s="4">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
       <c r="L24">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:27">
       <c r="A25" t="s">
         <v>36</v>
       </c>
+      <c r="B25" s="4">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
       <c r="P25">
         <v>14</v>
       </c>
@@ -1041,10 +1426,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:27">
       <c r="A26" t="s">
         <v>34</v>
       </c>
+      <c r="B26" s="4">
+        <f>SUM(C26:AA26)</f>
+        <v>60</v>
+      </c>
       <c r="L26">
         <v>7</v>
       </c>
@@ -1073,29 +1462,44 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:27">
       <c r="A27" t="s">
         <v>35</v>
       </c>
+      <c r="B27" s="4">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
       <c r="P27">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:27">
       <c r="A28" t="s">
         <v>37</v>
       </c>
+      <c r="B28" s="4">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
       <c r="Q28">
         <v>4</v>
       </c>
       <c r="R28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:25">
+      <c r="S28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27">
       <c r="A29" t="s">
         <v>38</v>
       </c>
+      <c r="B29" s="4">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
       <c r="R29">
         <v>3</v>
       </c>
@@ -1106,21 +1510,38 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:27">
       <c r="A30" t="s">
         <v>41</v>
       </c>
+      <c r="B30" s="4">
+        <f>SUM(C30:AA30)</f>
+        <v>17</v>
+      </c>
       <c r="W30">
         <v>6</v>
       </c>
       <c r="X30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:25">
+      <c r="Y30">
+        <v>2</v>
+      </c>
+      <c r="Z30">
+        <v>2</v>
+      </c>
+      <c r="AA30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27">
       <c r="A31" t="s">
         <v>42</v>
       </c>
+      <c r="B31" s="4">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
       <c r="W31">
         <v>6</v>
       </c>
@@ -1130,11 +1551,18 @@
       <c r="Y31">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:25">
+      <c r="Z31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27">
       <c r="A32" t="s">
         <v>44</v>
       </c>
+      <c r="B32" s="4">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
       <c r="W32">
         <v>6</v>
       </c>
@@ -1145,29 +1573,44 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:27">
       <c r="A33" t="s">
         <v>45</v>
       </c>
+      <c r="B33" s="4">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
       <c r="X33">
         <v>6</v>
       </c>
       <c r="Y33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:25">
+      <c r="Z33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27">
       <c r="A34" t="s">
         <v>43</v>
       </c>
+      <c r="B34" s="4">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
       <c r="W34">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:27">
       <c r="A35" t="s">
         <v>46</v>
       </c>
+      <c r="B35" s="4">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
       <c r="X35">
         <v>2</v>
       </c>
@@ -1175,25 +1618,92 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:27">
       <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="Z36">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="4">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="AA37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="4">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="AA38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="4">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="Z39">
+        <v>3</v>
+      </c>
+      <c r="AA39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="4">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="Z40">
+        <v>6</v>
+      </c>
+      <c r="AA40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27">
+      <c r="A41" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="30">
-      <c r="A40" s="3" t="s">
+    <row r="45" spans="1:27" ht="30">
+      <c r="A45" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="1:25">
-      <c r="A41" t="s">
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:27">
+      <c r="A46" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>